<commit_message>
Submit assignment 3 again
</commit_message>
<xml_diff>
--- a/Assignment3/TestDesign-Assignment3-QuynhAnh.xlsx
+++ b/Assignment3/TestDesign-Assignment3-QuynhAnh.xlsx
@@ -145,7 +145,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F132" authorId="1" shapeId="0">
+    <comment ref="F133" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -169,7 +169,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F141" authorId="1" shapeId="0">
+    <comment ref="F142" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F143" authorId="1" shapeId="0">
+    <comment ref="F144" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -222,7 +222,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="240">
   <si>
     <r>
       <t xml:space="preserve">Security Classification: </t>
@@ -1020,6 +1020,9 @@
   </si>
   <si>
     <t>Verify search is functional and generating the correct result for correct keywords by adding valid search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check if search box allows user to drag and drop images and files </t>
   </si>
 </sst>
 </file>
@@ -2740,41 +2743,86 @@
     <xf numFmtId="0" fontId="64" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="64" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="14" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="30" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="18" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="15" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="46" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="48" fillId="0" borderId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2782,6 +2830,15 @@
     <xf numFmtId="0" fontId="48" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="166" fontId="3" fillId="2" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="166" fontId="43" fillId="12" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -2791,65 +2848,11 @@
     <xf numFmtId="166" fontId="44" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="166" fontId="30" fillId="3" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="8" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="166" fontId="3" fillId="2" borderId="0" xfId="7" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="14" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="11" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="6" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="14" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="11" xfId="7" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="46" fillId="0" borderId="6" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="13" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="16" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="18" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="3" fillId="2" borderId="15" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="11" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -4666,10 +4669,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X143"/>
+  <dimension ref="A1:X144"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -4684,10 +4687,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="1" customFormat="1" ht="14.25">
-      <c r="A1" s="200"/>
-      <c r="B1" s="200"/>
-      <c r="C1" s="200"/>
-      <c r="D1" s="200"/>
+      <c r="A1" s="211"/>
+      <c r="B1" s="211"/>
+      <c r="C1" s="211"/>
+      <c r="D1" s="211"/>
       <c r="E1" s="34"/>
       <c r="F1" s="34"/>
       <c r="G1" s="34"/>
@@ -4696,13 +4699,13 @@
       <c r="J1" s="34"/>
     </row>
     <row r="2" spans="1:24" s="1" customFormat="1" ht="31.5" customHeight="1">
-      <c r="A2" s="201" t="s">
+      <c r="A2" s="212" t="s">
         <v>70</v>
       </c>
-      <c r="B2" s="201"/>
-      <c r="C2" s="201"/>
-      <c r="D2" s="201"/>
-      <c r="E2" s="210"/>
+      <c r="B2" s="212"/>
+      <c r="C2" s="212"/>
+      <c r="D2" s="212"/>
+      <c r="E2" s="207"/>
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -4711,9 +4714,9 @@
     </row>
     <row r="3" spans="1:24" s="1" customFormat="1" ht="31.5" customHeight="1">
       <c r="A3" s="47"/>
-      <c r="C3" s="211"/>
-      <c r="D3" s="211"/>
-      <c r="E3" s="210"/>
+      <c r="C3" s="208"/>
+      <c r="D3" s="208"/>
+      <c r="E3" s="207"/>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -4724,11 +4727,11 @@
       <c r="A4" s="135" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="203" t="s">
+      <c r="B4" s="209" t="s">
         <v>200</v>
       </c>
-      <c r="C4" s="203"/>
-      <c r="D4" s="203"/>
+      <c r="C4" s="209"/>
+      <c r="D4" s="209"/>
       <c r="E4" s="39"/>
       <c r="F4" s="39"/>
       <c r="G4" s="39"/>
@@ -4742,11 +4745,11 @@
       <c r="A5" s="135" t="s">
         <v>62</v>
       </c>
-      <c r="B5" s="202" t="s">
+      <c r="B5" s="210" t="s">
         <v>202</v>
       </c>
-      <c r="C5" s="203"/>
-      <c r="D5" s="203"/>
+      <c r="C5" s="209"/>
+      <c r="D5" s="209"/>
       <c r="E5" s="39"/>
       <c r="F5" s="39"/>
       <c r="G5" s="39"/>
@@ -4760,9 +4763,9 @@
       <c r="A6" s="135" t="s">
         <v>95</v>
       </c>
-      <c r="B6" s="202"/>
-      <c r="C6" s="203"/>
-      <c r="D6" s="203"/>
+      <c r="B6" s="210"/>
+      <c r="C6" s="209"/>
+      <c r="D6" s="209"/>
       <c r="E6" s="39"/>
       <c r="F6" s="39"/>
       <c r="G6" s="39"/>
@@ -4773,11 +4776,11 @@
       <c r="A7" s="135" t="s">
         <v>96</v>
       </c>
-      <c r="B7" s="203" t="s">
+      <c r="B7" s="209" t="s">
         <v>199</v>
       </c>
-      <c r="C7" s="203"/>
-      <c r="D7" s="203"/>
+      <c r="C7" s="209"/>
+      <c r="D7" s="209"/>
       <c r="E7" s="39"/>
       <c r="F7" s="39"/>
       <c r="G7" s="39"/>
@@ -4789,9 +4792,9 @@
       <c r="A8" s="135" t="s">
         <v>97</v>
       </c>
-      <c r="B8" s="204"/>
-      <c r="C8" s="204"/>
-      <c r="D8" s="204"/>
+      <c r="B8" s="213"/>
+      <c r="C8" s="213"/>
+      <c r="D8" s="213"/>
       <c r="E8" s="39"/>
     </row>
     <row r="9" spans="1:24" s="43" customFormat="1">
@@ -4833,15 +4836,15 @@
         <v>41</v>
       </c>
       <c r="B11" s="71">
-        <f>COUNTIF($F$19:$F$49695,"*Passed")</f>
+        <f>COUNTIF($F$19:$F$49696,"*Passed")</f>
         <v>0</v>
       </c>
       <c r="C11" s="71">
-        <f>COUNTIF($G$19:$G$49695,"*Passed")</f>
+        <f>COUNTIF($G$19:$G$49696,"*Passed")</f>
         <v>0</v>
       </c>
       <c r="D11" s="71">
-        <f>COUNTIF($H$19:$H$49695,"*Passed")</f>
+        <f>COUNTIF($H$19:$H$49696,"*Passed")</f>
         <v>0</v>
       </c>
     </row>
@@ -4850,15 +4853,15 @@
         <v>43</v>
       </c>
       <c r="B12" s="71">
-        <f>COUNTIF($F$19:$F$49415,"*Failed*")</f>
+        <f>COUNTIF($F$19:$F$49416,"*Failed*")</f>
         <v>0</v>
       </c>
       <c r="C12" s="71">
-        <f>COUNTIF($G$19:$G$49415,"*Failed*")</f>
+        <f>COUNTIF($G$19:$G$49416,"*Failed*")</f>
         <v>0</v>
       </c>
       <c r="D12" s="71">
-        <f>COUNTIF($H$19:$H$49415,"*Failed*")</f>
+        <f>COUNTIF($H$19:$H$49416,"*Failed*")</f>
         <v>0</v>
       </c>
     </row>
@@ -4867,15 +4870,15 @@
         <v>45</v>
       </c>
       <c r="B13" s="71">
-        <f>COUNTIF($F$19:$F$49415,"*Not Run*")</f>
+        <f>COUNTIF($F$19:$F$49416,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="C13" s="71">
-        <f>COUNTIF($G$19:$G$49415,"*Not Run*")</f>
+        <f>COUNTIF($G$19:$G$49416,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="D13" s="71">
-        <f>COUNTIF($H$19:$H$49415,"*Not Run*")</f>
+        <f>COUNTIF($H$19:$H$49416,"*Not Run*")</f>
         <v>0</v>
       </c>
       <c r="E13" s="1"/>
@@ -4889,15 +4892,15 @@
         <v>100</v>
       </c>
       <c r="B14" s="71">
-        <f>COUNTIF($F$19:$F$49415,"*NA*")</f>
+        <f>COUNTIF($F$19:$F$49416,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="C14" s="71">
-        <f>COUNTIF($G$19:$G$49415,"*NA*")</f>
+        <f>COUNTIF($G$19:$G$49416,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="D14" s="71">
-        <f>COUNTIF($H$19:$H$49415,"*NA*")</f>
+        <f>COUNTIF($H$19:$H$49416,"*NA*")</f>
         <v>0</v>
       </c>
       <c r="E14" s="1"/>
@@ -4911,15 +4914,15 @@
         <v>101</v>
       </c>
       <c r="B15" s="71">
-        <f>COUNTIF($F$19:$F$49415,"*Passed in previous build*")</f>
+        <f>COUNTIF($F$19:$F$49416,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="C15" s="71">
-        <f>COUNTIF($G$19:$G$49415,"*Passed in previous build*")</f>
+        <f>COUNTIF($G$19:$G$49416,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="D15" s="71">
-        <f>COUNTIF($H$19:$H$49415,"*Passed in previous build*")</f>
+        <f>COUNTIF($H$19:$H$49416,"*Passed in previous build*")</f>
         <v>0</v>
       </c>
       <c r="E15" s="1"/>
@@ -4934,11 +4937,11 @@
       <c r="C16" s="49"/>
       <c r="D16" s="50"/>
       <c r="E16" s="55"/>
-      <c r="F16" s="205" t="s">
+      <c r="F16" s="200" t="s">
         <v>98</v>
       </c>
-      <c r="G16" s="205"/>
-      <c r="H16" s="205"/>
+      <c r="G16" s="200"/>
+      <c r="H16" s="200"/>
       <c r="I16" s="56"/>
     </row>
     <row r="17" spans="1:9" s="44" customFormat="1" ht="38.25">
@@ -4972,11 +4975,11 @@
     </row>
     <row r="18" spans="1:9" s="44" customFormat="1" ht="15.75" customHeight="1">
       <c r="A18" s="63"/>
-      <c r="B18" s="206" t="s">
+      <c r="B18" s="201" t="s">
         <v>201</v>
       </c>
-      <c r="C18" s="207"/>
-      <c r="D18" s="208"/>
+      <c r="C18" s="205"/>
+      <c r="D18" s="206"/>
       <c r="E18" s="63"/>
       <c r="F18" s="64"/>
       <c r="G18" s="64"/>
@@ -4985,11 +4988,11 @@
     </row>
     <row r="19" spans="1:9" s="44" customFormat="1" ht="15.75" customHeight="1">
       <c r="A19" s="63"/>
-      <c r="B19" s="206" t="s">
+      <c r="B19" s="201" t="s">
         <v>203</v>
       </c>
-      <c r="C19" s="235"/>
-      <c r="D19" s="236"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="203"/>
       <c r="E19" s="63"/>
       <c r="F19" s="64"/>
       <c r="G19" s="64"/>
@@ -5013,7 +5016,7 @@
     </row>
     <row r="21" spans="1:9" s="45" customFormat="1">
       <c r="A21" s="57">
-        <f ca="1">IF(OFFSET(A21,-1,0) ="",OFFSET(A21,-2,0)+1,OFFSET(A21,-1,0)+1 )</f>
+        <f t="shared" ref="A21:A28" ca="1" si="0">IF(OFFSET(A21,-1,0) ="",OFFSET(A21,-2,0)+1,OFFSET(A21,-1,0)+1 )</f>
         <v>2</v>
       </c>
       <c r="B21" s="51" t="s">
@@ -5029,7 +5032,7 @@
     </row>
     <row r="22" spans="1:9" s="45" customFormat="1" ht="25.5">
       <c r="A22" s="57">
-        <f ca="1">IF(OFFSET(A22,-1,0) ="",OFFSET(A22,-2,0)+1,OFFSET(A22,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>3</v>
       </c>
       <c r="B22" s="51" t="s">
@@ -5045,7 +5048,7 @@
     </row>
     <row r="23" spans="1:9" s="45" customFormat="1" ht="25.5">
       <c r="A23" s="57">
-        <f ca="1">IF(OFFSET(A23,-1,0) ="",OFFSET(A23,-2,0)+1,OFFSET(A23,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>4</v>
       </c>
       <c r="B23" s="51" t="s">
@@ -5061,7 +5064,7 @@
     </row>
     <row r="24" spans="1:9" s="45" customFormat="1">
       <c r="A24" s="57">
-        <f ca="1">IF(OFFSET(A24,-1,0) ="",OFFSET(A24,-2,0)+1,OFFSET(A24,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>5</v>
       </c>
       <c r="B24" s="51" t="s">
@@ -5077,7 +5080,7 @@
     </row>
     <row r="25" spans="1:9" s="45" customFormat="1">
       <c r="A25" s="57">
-        <f ca="1">IF(OFFSET(A25,-1,0) ="",OFFSET(A25,-2,0)+1,OFFSET(A25,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>6</v>
       </c>
       <c r="B25" s="51" t="s">
@@ -5091,61 +5094,61 @@
       <c r="H25" s="51"/>
       <c r="I25" s="54"/>
     </row>
-    <row r="26" spans="1:9" s="48" customFormat="1" ht="14.25">
+    <row r="26" spans="1:9" s="45" customFormat="1">
       <c r="A26" s="57">
-        <f ca="1">IF(OFFSET(A26,-1,0) ="",OFFSET(A26,-2,0)+1,OFFSET(A26,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>7</v>
       </c>
       <c r="B26" s="51" t="s">
-        <v>209</v>
+        <v>239</v>
       </c>
       <c r="C26" s="51"/>
-      <c r="D26" s="53"/>
+      <c r="D26" s="59"/>
       <c r="E26" s="53"/>
       <c r="F26" s="51"/>
       <c r="G26" s="51"/>
       <c r="H26" s="51"/>
-      <c r="I26" s="60"/>
-    </row>
-    <row r="27" spans="1:9" s="48" customFormat="1" ht="25.5">
+      <c r="I26" s="54"/>
+    </row>
+    <row r="27" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A27" s="57">
-        <f ca="1">IF(OFFSET(A27,-1,0) ="",OFFSET(A27,-2,0)+1,OFFSET(A27,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>8</v>
       </c>
       <c r="B27" s="51" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C27" s="51"/>
-      <c r="D27" s="59"/>
+      <c r="D27" s="53"/>
       <c r="E27" s="53"/>
       <c r="F27" s="51"/>
       <c r="G27" s="51"/>
       <c r="H27" s="51"/>
       <c r="I27" s="60"/>
     </row>
-    <row r="28" spans="1:9" s="48" customFormat="1" ht="14.25">
+    <row r="28" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A28" s="57">
-        <f t="shared" ref="A28:A135" ca="1" si="0">IF(OFFSET(A28,-1,0) ="",OFFSET(A28,-2,0)+1,OFFSET(A28,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="0"/>
         <v>9</v>
       </c>
       <c r="B28" s="51" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C28" s="51"/>
-      <c r="D28" s="53"/>
+      <c r="D28" s="59"/>
       <c r="E28" s="53"/>
       <c r="F28" s="51"/>
       <c r="G28" s="51"/>
       <c r="H28" s="51"/>
       <c r="I28" s="60"/>
     </row>
-    <row r="29" spans="1:9" s="48" customFormat="1" ht="25.5">
+    <row r="29" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A29" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ref="A29:A136" ca="1" si="1">IF(OFFSET(A29,-1,0) ="",OFFSET(A29,-2,0)+1,OFFSET(A29,-1,0)+1 )</f>
         <v>10</v>
       </c>
       <c r="B29" s="51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C29" s="51"/>
       <c r="D29" s="53"/>
@@ -5155,13 +5158,13 @@
       <c r="H29" s="51"/>
       <c r="I29" s="60"/>
     </row>
-    <row r="30" spans="1:9" s="48" customFormat="1" ht="14.25">
+    <row r="30" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A30" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>11</v>
       </c>
       <c r="B30" s="51" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C30" s="51"/>
       <c r="D30" s="53"/>
@@ -5171,13 +5174,13 @@
       <c r="H30" s="51"/>
       <c r="I30" s="60"/>
     </row>
-    <row r="31" spans="1:9" s="48" customFormat="1" ht="25.5">
+    <row r="31" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A31" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>12</v>
       </c>
       <c r="B31" s="51" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="C31" s="51"/>
       <c r="D31" s="53"/>
@@ -5187,13 +5190,13 @@
       <c r="H31" s="51"/>
       <c r="I31" s="60"/>
     </row>
-    <row r="32" spans="1:9" s="48" customFormat="1" ht="14.25">
+    <row r="32" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A32" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>13</v>
       </c>
       <c r="B32" s="51" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C32" s="51"/>
       <c r="D32" s="53"/>
@@ -5205,11 +5208,11 @@
     </row>
     <row r="33" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A33" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>14</v>
       </c>
       <c r="B33" s="51" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C33" s="51"/>
       <c r="D33" s="53"/>
@@ -5221,11 +5224,11 @@
     </row>
     <row r="34" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A34" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>15</v>
       </c>
       <c r="B34" s="51" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C34" s="51"/>
       <c r="D34" s="53"/>
@@ -5237,11 +5240,11 @@
     </row>
     <row r="35" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A35" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>16</v>
       </c>
       <c r="B35" s="51" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C35" s="51"/>
       <c r="D35" s="53"/>
@@ -5253,11 +5256,11 @@
     </row>
     <row r="36" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A36" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>17</v>
       </c>
       <c r="B36" s="51" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C36" s="51"/>
       <c r="D36" s="53"/>
@@ -5267,13 +5270,13 @@
       <c r="H36" s="51"/>
       <c r="I36" s="60"/>
     </row>
-    <row r="37" spans="1:9" s="48" customFormat="1" ht="25.5">
+    <row r="37" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A37" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>18</v>
       </c>
       <c r="B37" s="51" t="s">
-        <v>237</v>
+        <v>220</v>
       </c>
       <c r="C37" s="51"/>
       <c r="D37" s="53"/>
@@ -5285,11 +5288,11 @@
     </row>
     <row r="38" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A38" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>19</v>
       </c>
       <c r="B38" s="51" t="s">
-        <v>221</v>
+        <v>237</v>
       </c>
       <c r="C38" s="51"/>
       <c r="D38" s="53"/>
@@ -5299,13 +5302,13 @@
       <c r="H38" s="51"/>
       <c r="I38" s="60"/>
     </row>
-    <row r="39" spans="1:9" s="48" customFormat="1" ht="14.25">
+    <row r="39" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A39" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>20</v>
       </c>
       <c r="B39" s="51" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C39" s="51"/>
       <c r="D39" s="53"/>
@@ -5315,13 +5318,13 @@
       <c r="H39" s="51"/>
       <c r="I39" s="60"/>
     </row>
-    <row r="40" spans="1:9" s="48" customFormat="1" ht="38.25">
+    <row r="40" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A40" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>21</v>
       </c>
       <c r="B40" s="51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C40" s="51"/>
       <c r="D40" s="53"/>
@@ -5331,13 +5334,13 @@
       <c r="H40" s="51"/>
       <c r="I40" s="60"/>
     </row>
-    <row r="41" spans="1:9" s="48" customFormat="1" ht="14.25">
+    <row r="41" spans="1:9" s="48" customFormat="1" ht="38.25">
       <c r="A41" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>22</v>
       </c>
       <c r="B41" s="51" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C41" s="51"/>
       <c r="D41" s="53"/>
@@ -5349,11 +5352,11 @@
     </row>
     <row r="42" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A42" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>23</v>
       </c>
       <c r="B42" s="51" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C42" s="51"/>
       <c r="D42" s="53"/>
@@ -5365,11 +5368,11 @@
     </row>
     <row r="43" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A43" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>24</v>
       </c>
       <c r="B43" s="51" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C43" s="51"/>
       <c r="D43" s="53"/>
@@ -5379,13 +5382,13 @@
       <c r="H43" s="51"/>
       <c r="I43" s="60"/>
     </row>
-    <row r="44" spans="1:9" s="48" customFormat="1" ht="25.5">
+    <row r="44" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A44" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>25</v>
       </c>
       <c r="B44" s="51" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C44" s="51"/>
       <c r="D44" s="53"/>
@@ -5397,11 +5400,11 @@
     </row>
     <row r="45" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A45" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>26</v>
       </c>
       <c r="B45" s="51" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C45" s="51"/>
       <c r="D45" s="53"/>
@@ -5413,11 +5416,11 @@
     </row>
     <row r="46" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A46" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>27</v>
       </c>
       <c r="B46" s="51" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="C46" s="51"/>
       <c r="D46" s="53"/>
@@ -5429,11 +5432,11 @@
     </row>
     <row r="47" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A47" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>28</v>
       </c>
       <c r="B47" s="51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C47" s="51"/>
       <c r="D47" s="53"/>
@@ -5445,11 +5448,11 @@
     </row>
     <row r="48" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A48" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>29</v>
       </c>
       <c r="B48" s="51" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C48" s="51"/>
       <c r="D48" s="53"/>
@@ -5461,11 +5464,11 @@
     </row>
     <row r="49" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A49" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>30</v>
       </c>
       <c r="B49" s="51" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C49" s="51"/>
       <c r="D49" s="53"/>
@@ -5477,7 +5480,7 @@
     </row>
     <row r="50" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A50" s="57">
-        <f ca="1">IF(OFFSET(A50,-1,0) ="",OFFSET(A50,-2,0)+1,OFFSET(A50,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="1"/>
         <v>31</v>
       </c>
       <c r="B50" s="51" t="s">
@@ -5493,7 +5496,7 @@
     </row>
     <row r="51" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A51" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A51,-1,0) ="",OFFSET(A51,-2,0)+1,OFFSET(A51,-1,0)+1 )</f>
         <v>32</v>
       </c>
       <c r="B51" s="51" t="s">
@@ -5509,11 +5512,11 @@
     </row>
     <row r="52" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A52" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>33</v>
       </c>
       <c r="B52" s="51" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C52" s="51"/>
       <c r="D52" s="53"/>
@@ -5523,13 +5526,13 @@
       <c r="H52" s="51"/>
       <c r="I52" s="60"/>
     </row>
-    <row r="53" spans="1:9" s="48" customFormat="1" ht="14.25">
+    <row r="53" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A53" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>34</v>
       </c>
       <c r="B53" s="51" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C53" s="51"/>
       <c r="D53" s="53"/>
@@ -5539,13 +5542,13 @@
       <c r="H53" s="51"/>
       <c r="I53" s="60"/>
     </row>
-    <row r="54" spans="1:9" s="48" customFormat="1" ht="25.5">
+    <row r="54" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A54" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>35</v>
       </c>
       <c r="B54" s="51" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C54" s="51"/>
       <c r="D54" s="53"/>
@@ -5555,13 +5558,13 @@
       <c r="H54" s="51"/>
       <c r="I54" s="60"/>
     </row>
-    <row r="55" spans="1:9" s="48" customFormat="1" ht="14.25">
+    <row r="55" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A55" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>36</v>
       </c>
       <c r="B55" s="51" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C55" s="51"/>
       <c r="D55" s="53"/>
@@ -5571,13 +5574,13 @@
       <c r="H55" s="51"/>
       <c r="I55" s="60"/>
     </row>
-    <row r="56" spans="1:9" s="48" customFormat="1" ht="25.5">
+    <row r="56" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A56" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>37</v>
       </c>
       <c r="B56" s="51" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C56" s="51"/>
       <c r="D56" s="53"/>
@@ -5587,12 +5590,14 @@
       <c r="H56" s="51"/>
       <c r="I56" s="60"/>
     </row>
-    <row r="57" spans="1:9" s="48" customFormat="1" ht="14.25">
+    <row r="57" spans="1:9" s="48" customFormat="1" ht="25.5">
       <c r="A57" s="57">
-        <f ca="1">IF(OFFSET(A57,-1,0) ="",OFFSET(A57,-2,0)+1,OFFSET(A57,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="1"/>
         <v>38</v>
       </c>
-      <c r="B57" s="51"/>
+      <c r="B57" s="51" t="s">
+        <v>238</v>
+      </c>
       <c r="C57" s="51"/>
       <c r="D57" s="53"/>
       <c r="E57" s="53"/>
@@ -5603,7 +5608,7 @@
     </row>
     <row r="58" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A58" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A58,-1,0) ="",OFFSET(A58,-2,0)+1,OFFSET(A58,-1,0)+1 )</f>
         <v>39</v>
       </c>
       <c r="B58" s="51"/>
@@ -5617,7 +5622,7 @@
     </row>
     <row r="59" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A59" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>40</v>
       </c>
       <c r="B59" s="51"/>
@@ -5631,7 +5636,7 @@
     </row>
     <row r="60" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A60" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>41</v>
       </c>
       <c r="B60" s="51"/>
@@ -5645,7 +5650,7 @@
     </row>
     <row r="61" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A61" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>42</v>
       </c>
       <c r="B61" s="51"/>
@@ -5659,7 +5664,7 @@
     </row>
     <row r="62" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A62" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>43</v>
       </c>
       <c r="B62" s="51"/>
@@ -5673,7 +5678,7 @@
     </row>
     <row r="63" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A63" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>44</v>
       </c>
       <c r="B63" s="51"/>
@@ -5687,7 +5692,7 @@
     </row>
     <row r="64" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A64" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>45</v>
       </c>
       <c r="B64" s="51"/>
@@ -5701,7 +5706,7 @@
     </row>
     <row r="65" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A65" s="57">
-        <f ca="1">IF(OFFSET(A65,-1,0) ="",OFFSET(A65,-2,0)+1,OFFSET(A65,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="1"/>
         <v>46</v>
       </c>
       <c r="B65" s="51"/>
@@ -5715,7 +5720,7 @@
     </row>
     <row r="66" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A66" s="57">
-        <f t="shared" ref="A66:A68" ca="1" si="1">IF(OFFSET(A66,-1,0) ="",OFFSET(A66,-2,0)+1,OFFSET(A66,-1,0)+1 )</f>
+        <f ca="1">IF(OFFSET(A66,-1,0) ="",OFFSET(A66,-2,0)+1,OFFSET(A66,-1,0)+1 )</f>
         <v>47</v>
       </c>
       <c r="B66" s="51"/>
@@ -5729,7 +5734,7 @@
     </row>
     <row r="67" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A67" s="57">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ref="A67:A69" ca="1" si="2">IF(OFFSET(A67,-1,0) ="",OFFSET(A67,-2,0)+1,OFFSET(A67,-1,0)+1 )</f>
         <v>48</v>
       </c>
       <c r="B67" s="51"/>
@@ -5743,7 +5748,7 @@
     </row>
     <row r="68" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A68" s="57">
-        <f t="shared" ca="1" si="1"/>
+        <f t="shared" ca="1" si="2"/>
         <v>49</v>
       </c>
       <c r="B68" s="51"/>
@@ -5755,33 +5760,33 @@
       <c r="H68" s="51"/>
       <c r="I68" s="60"/>
     </row>
-    <row r="69" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B69" s="162"/>
-      <c r="C69" s="163"/>
-      <c r="D69" s="164"/>
-      <c r="E69" s="162"/>
-      <c r="F69" s="165"/>
-      <c r="G69" s="165"/>
-      <c r="H69" s="165"/>
-      <c r="I69" s="162"/>
-    </row>
-    <row r="70" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A70" s="57">
-        <f ca="1">IF(OFFSET(A70,-1,0) ="",OFFSET(A70,-2,0)+1,OFFSET(A70,-1,0)+1 )</f>
+    <row r="69" spans="1:9" s="48" customFormat="1" ht="14.25">
+      <c r="A69" s="57">
+        <f t="shared" ca="1" si="2"/>
         <v>50</v>
       </c>
-      <c r="B70" s="51"/>
-      <c r="C70" s="51"/>
-      <c r="D70" s="53"/>
-      <c r="E70" s="53"/>
-      <c r="F70" s="51"/>
-      <c r="G70" s="51"/>
-      <c r="H70" s="51"/>
-      <c r="I70" s="60"/>
+      <c r="B69" s="51"/>
+      <c r="C69" s="51"/>
+      <c r="D69" s="53"/>
+      <c r="E69" s="53"/>
+      <c r="F69" s="51"/>
+      <c r="G69" s="51"/>
+      <c r="H69" s="51"/>
+      <c r="I69" s="60"/>
+    </row>
+    <row r="70" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B70" s="162"/>
+      <c r="C70" s="163"/>
+      <c r="D70" s="164"/>
+      <c r="E70" s="162"/>
+      <c r="F70" s="165"/>
+      <c r="G70" s="165"/>
+      <c r="H70" s="165"/>
+      <c r="I70" s="162"/>
     </row>
     <row r="71" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A71" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A71,-1,0) ="",OFFSET(A71,-2,0)+1,OFFSET(A71,-1,0)+1 )</f>
         <v>51</v>
       </c>
       <c r="B71" s="51"/>
@@ -5795,7 +5800,7 @@
     </row>
     <row r="72" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A72" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>52</v>
       </c>
       <c r="B72" s="51"/>
@@ -5809,10 +5814,11 @@
     </row>
     <row r="73" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A73" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>53</v>
       </c>
       <c r="B73" s="51"/>
+      <c r="C73" s="51"/>
       <c r="D73" s="53"/>
       <c r="E73" s="53"/>
       <c r="F73" s="51"/>
@@ -5822,11 +5828,10 @@
     </row>
     <row r="74" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A74" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>54</v>
       </c>
       <c r="B74" s="51"/>
-      <c r="C74" s="51"/>
       <c r="D74" s="53"/>
       <c r="E74" s="53"/>
       <c r="F74" s="51"/>
@@ -5836,7 +5841,7 @@
     </row>
     <row r="75" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A75" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>55</v>
       </c>
       <c r="B75" s="51"/>
@@ -5850,7 +5855,7 @@
     </row>
     <row r="76" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A76" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>56</v>
       </c>
       <c r="B76" s="51"/>
@@ -5864,7 +5869,7 @@
     </row>
     <row r="77" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A77" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>57</v>
       </c>
       <c r="B77" s="51"/>
@@ -5878,7 +5883,7 @@
     </row>
     <row r="78" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A78" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>58</v>
       </c>
       <c r="B78" s="51"/>
@@ -5892,7 +5897,7 @@
     </row>
     <row r="79" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A79" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>59</v>
       </c>
       <c r="B79" s="51"/>
@@ -5906,7 +5911,7 @@
     </row>
     <row r="80" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A80" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>60</v>
       </c>
       <c r="B80" s="51"/>
@@ -5920,7 +5925,7 @@
     </row>
     <row r="81" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A81" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>61</v>
       </c>
       <c r="B81" s="51"/>
@@ -5934,7 +5939,7 @@
     </row>
     <row r="82" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A82" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>62</v>
       </c>
       <c r="B82" s="51"/>
@@ -5948,7 +5953,7 @@
     </row>
     <row r="83" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A83" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>63</v>
       </c>
       <c r="B83" s="51"/>
@@ -5962,7 +5967,7 @@
     </row>
     <row r="84" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A84" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>64</v>
       </c>
       <c r="B84" s="51"/>
@@ -5976,7 +5981,7 @@
     </row>
     <row r="85" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A85" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>65</v>
       </c>
       <c r="B85" s="51"/>
@@ -5990,7 +5995,7 @@
     </row>
     <row r="86" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A86" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>66</v>
       </c>
       <c r="B86" s="51"/>
@@ -6002,36 +6007,36 @@
       <c r="H86" s="51"/>
       <c r="I86" s="60"/>
     </row>
-    <row r="87" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B87" s="162"/>
-      <c r="C87" s="163"/>
-      <c r="D87" s="164"/>
-      <c r="E87" s="162"/>
-      <c r="F87" s="165"/>
-      <c r="G87" s="165"/>
-      <c r="H87" s="165"/>
-      <c r="I87" s="162"/>
-    </row>
-    <row r="88" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A88" s="57">
-        <f t="shared" ca="1" si="0"/>
+    <row r="87" spans="1:9" s="48" customFormat="1" ht="14.25">
+      <c r="A87" s="57">
+        <f t="shared" ca="1" si="1"/>
         <v>67</v>
       </c>
-      <c r="B88" s="51"/>
-      <c r="D88" s="53"/>
-      <c r="E88" s="53"/>
-      <c r="F88" s="51"/>
-      <c r="G88" s="51"/>
-      <c r="H88" s="51"/>
-      <c r="I88" s="60"/>
+      <c r="B87" s="51"/>
+      <c r="C87" s="51"/>
+      <c r="D87" s="53"/>
+      <c r="E87" s="53"/>
+      <c r="F87" s="51"/>
+      <c r="G87" s="51"/>
+      <c r="H87" s="51"/>
+      <c r="I87" s="60"/>
+    </row>
+    <row r="88" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B88" s="162"/>
+      <c r="C88" s="163"/>
+      <c r="D88" s="164"/>
+      <c r="E88" s="162"/>
+      <c r="F88" s="165"/>
+      <c r="G88" s="165"/>
+      <c r="H88" s="165"/>
+      <c r="I88" s="162"/>
     </row>
     <row r="89" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A89" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>68</v>
       </c>
       <c r="B89" s="51"/>
-      <c r="C89" s="51"/>
       <c r="D89" s="53"/>
       <c r="E89" s="53"/>
       <c r="F89" s="51"/>
@@ -6041,7 +6046,7 @@
     </row>
     <row r="90" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A90" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>69</v>
       </c>
       <c r="B90" s="51"/>
@@ -6055,7 +6060,7 @@
     </row>
     <row r="91" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A91" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>70</v>
       </c>
       <c r="B91" s="51"/>
@@ -6069,7 +6074,7 @@
     </row>
     <row r="92" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A92" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>71</v>
       </c>
       <c r="B92" s="51"/>
@@ -6083,7 +6088,7 @@
     </row>
     <row r="93" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A93" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>72</v>
       </c>
       <c r="B93" s="51"/>
@@ -6097,7 +6102,7 @@
     </row>
     <row r="94" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A94" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>73</v>
       </c>
       <c r="B94" s="51"/>
@@ -6109,47 +6114,47 @@
       <c r="H94" s="51"/>
       <c r="I94" s="60"/>
     </row>
-    <row r="95" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B95" s="162"/>
-      <c r="C95" s="163"/>
-      <c r="D95" s="164"/>
-      <c r="E95" s="162"/>
-      <c r="F95" s="165"/>
-      <c r="G95" s="165"/>
-      <c r="H95" s="165"/>
-      <c r="I95" s="162"/>
-    </row>
-    <row r="96" spans="1:9" s="169" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A96" s="57">
-        <f t="shared" ca="1" si="0"/>
+    <row r="95" spans="1:9" s="48" customFormat="1" ht="14.25">
+      <c r="A95" s="57">
+        <f t="shared" ca="1" si="1"/>
         <v>74</v>
       </c>
-      <c r="B96" s="51"/>
-      <c r="C96" s="171"/>
-      <c r="D96" s="172"/>
-      <c r="E96" s="170"/>
-      <c r="F96" s="173"/>
-      <c r="G96" s="173"/>
-      <c r="H96" s="173"/>
-      <c r="I96" s="170"/>
-    </row>
-    <row r="97" spans="1:9" s="48" customFormat="1" ht="14.25">
+      <c r="B95" s="51"/>
+      <c r="C95" s="51"/>
+      <c r="D95" s="53"/>
+      <c r="E95" s="53"/>
+      <c r="F95" s="51"/>
+      <c r="G95" s="51"/>
+      <c r="H95" s="51"/>
+      <c r="I95" s="60"/>
+    </row>
+    <row r="96" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B96" s="162"/>
+      <c r="C96" s="163"/>
+      <c r="D96" s="164"/>
+      <c r="E96" s="162"/>
+      <c r="F96" s="165"/>
+      <c r="G96" s="165"/>
+      <c r="H96" s="165"/>
+      <c r="I96" s="162"/>
+    </row>
+    <row r="97" spans="1:9" s="169" customFormat="1" ht="15.75" customHeight="1">
       <c r="A97" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>75</v>
       </c>
       <c r="B97" s="51"/>
-      <c r="C97" s="51"/>
-      <c r="D97" s="53"/>
-      <c r="E97" s="53"/>
-      <c r="F97" s="51"/>
-      <c r="G97" s="51"/>
-      <c r="H97" s="51"/>
-      <c r="I97" s="60"/>
+      <c r="C97" s="171"/>
+      <c r="D97" s="172"/>
+      <c r="E97" s="170"/>
+      <c r="F97" s="173"/>
+      <c r="G97" s="173"/>
+      <c r="H97" s="173"/>
+      <c r="I97" s="170"/>
     </row>
     <row r="98" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A98" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>76</v>
       </c>
       <c r="B98" s="51"/>
@@ -6163,7 +6168,7 @@
     </row>
     <row r="99" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A99" s="57">
-        <f ca="1">IF(OFFSET(A99,-1,0) ="",OFFSET(A99,-2,0)+1,OFFSET(A99,-1,0)+1 )</f>
+        <f t="shared" ca="1" si="1"/>
         <v>77</v>
       </c>
       <c r="B99" s="51"/>
@@ -6177,7 +6182,7 @@
     </row>
     <row r="100" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A100" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f ca="1">IF(OFFSET(A100,-1,0) ="",OFFSET(A100,-2,0)+1,OFFSET(A100,-1,0)+1 )</f>
         <v>78</v>
       </c>
       <c r="B100" s="51"/>
@@ -6191,7 +6196,7 @@
     </row>
     <row r="101" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A101" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>79</v>
       </c>
       <c r="B101" s="51"/>
@@ -6205,7 +6210,7 @@
     </row>
     <row r="102" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A102" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>80</v>
       </c>
       <c r="B102" s="51"/>
@@ -6219,7 +6224,7 @@
     </row>
     <row r="103" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A103" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>81</v>
       </c>
       <c r="B103" s="51"/>
@@ -6233,7 +6238,7 @@
     </row>
     <row r="104" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A104" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>82</v>
       </c>
       <c r="B104" s="51"/>
@@ -6247,7 +6252,7 @@
     </row>
     <row r="105" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A105" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>83</v>
       </c>
       <c r="B105" s="51"/>
@@ -6261,7 +6266,7 @@
     </row>
     <row r="106" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A106" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>84</v>
       </c>
       <c r="B106" s="51"/>
@@ -6275,7 +6280,7 @@
     </row>
     <row r="107" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A107" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>85</v>
       </c>
       <c r="B107" s="51"/>
@@ -6289,45 +6294,45 @@
     </row>
     <row r="108" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A108" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>86</v>
       </c>
       <c r="B108" s="51"/>
-      <c r="C108" s="167"/>
-      <c r="D108" s="168"/>
+      <c r="C108" s="51"/>
+      <c r="D108" s="53"/>
       <c r="E108" s="53"/>
       <c r="F108" s="51"/>
       <c r="G108" s="51"/>
       <c r="H108" s="51"/>
       <c r="I108" s="60"/>
     </row>
-    <row r="109" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B109" s="162"/>
-      <c r="C109" s="163"/>
-      <c r="D109" s="164"/>
-      <c r="E109" s="162"/>
-      <c r="F109" s="165"/>
-      <c r="G109" s="165"/>
-      <c r="H109" s="165"/>
-      <c r="I109" s="162"/>
-    </row>
-    <row r="110" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A110" s="57">
-        <f t="shared" ca="1" si="0"/>
+    <row r="109" spans="1:9" s="48" customFormat="1" ht="14.25">
+      <c r="A109" s="57">
+        <f t="shared" ca="1" si="1"/>
         <v>87</v>
       </c>
-      <c r="B110" s="51"/>
-      <c r="C110" s="51"/>
-      <c r="D110" s="53"/>
-      <c r="E110" s="53"/>
-      <c r="F110" s="51"/>
-      <c r="G110" s="51"/>
-      <c r="H110" s="51"/>
-      <c r="I110" s="60"/>
+      <c r="B109" s="51"/>
+      <c r="C109" s="167"/>
+      <c r="D109" s="168"/>
+      <c r="E109" s="53"/>
+      <c r="F109" s="51"/>
+      <c r="G109" s="51"/>
+      <c r="H109" s="51"/>
+      <c r="I109" s="60"/>
+    </row>
+    <row r="110" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B110" s="162"/>
+      <c r="C110" s="163"/>
+      <c r="D110" s="164"/>
+      <c r="E110" s="162"/>
+      <c r="F110" s="165"/>
+      <c r="G110" s="165"/>
+      <c r="H110" s="165"/>
+      <c r="I110" s="162"/>
     </row>
     <row r="111" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A111" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>88</v>
       </c>
       <c r="B111" s="51"/>
@@ -6341,7 +6346,7 @@
     </row>
     <row r="112" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A112" s="57">
-        <f t="shared" ca="1" si="0"/>
+        <f t="shared" ca="1" si="1"/>
         <v>89</v>
       </c>
       <c r="B112" s="51"/>
@@ -6354,43 +6359,43 @@
       <c r="I112" s="60"/>
     </row>
     <row r="113" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A113" s="73"/>
-      <c r="B113" s="209"/>
-      <c r="C113" s="207"/>
-      <c r="D113" s="208"/>
-      <c r="E113" s="65"/>
-      <c r="F113" s="62"/>
-      <c r="G113" s="62"/>
-      <c r="H113" s="62"/>
-      <c r="I113" s="65"/>
-    </row>
-    <row r="114" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B114" s="162"/>
-      <c r="C114" s="163"/>
-      <c r="D114" s="164"/>
-      <c r="E114" s="162"/>
-      <c r="F114" s="165"/>
-      <c r="G114" s="165"/>
-      <c r="H114" s="165"/>
-      <c r="I114" s="162"/>
-    </row>
-    <row r="115" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A115" s="61">
-        <v>73</v>
-      </c>
-      <c r="B115" s="51"/>
-      <c r="C115" s="51"/>
-      <c r="D115" s="53"/>
-      <c r="E115" s="53"/>
-      <c r="F115" s="51"/>
-      <c r="G115" s="51"/>
-      <c r="H115" s="51"/>
-      <c r="I115" s="61"/>
+      <c r="A113" s="57">
+        <f t="shared" ca="1" si="1"/>
+        <v>90</v>
+      </c>
+      <c r="B113" s="51"/>
+      <c r="C113" s="51"/>
+      <c r="D113" s="53"/>
+      <c r="E113" s="53"/>
+      <c r="F113" s="51"/>
+      <c r="G113" s="51"/>
+      <c r="H113" s="51"/>
+      <c r="I113" s="60"/>
+    </row>
+    <row r="114" spans="1:9" s="48" customFormat="1" ht="14.25">
+      <c r="A114" s="73"/>
+      <c r="B114" s="204"/>
+      <c r="C114" s="205"/>
+      <c r="D114" s="206"/>
+      <c r="E114" s="65"/>
+      <c r="F114" s="62"/>
+      <c r="G114" s="62"/>
+      <c r="H114" s="62"/>
+      <c r="I114" s="65"/>
+    </row>
+    <row r="115" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B115" s="162"/>
+      <c r="C115" s="163"/>
+      <c r="D115" s="164"/>
+      <c r="E115" s="162"/>
+      <c r="F115" s="165"/>
+      <c r="G115" s="165"/>
+      <c r="H115" s="165"/>
+      <c r="I115" s="162"/>
     </row>
     <row r="116" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A116" s="61">
-        <f t="shared" ref="A116:A128" ca="1" si="2">IF(OFFSET(A116,-1,0) ="",OFFSET(A116,-2,0)+1,OFFSET(A116,-1,0)+1 )</f>
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B116" s="51"/>
       <c r="C116" s="51"/>
@@ -6403,13 +6408,13 @@
     </row>
     <row r="117" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A117" s="61">
-        <f t="shared" ca="1" si="2"/>
-        <v>75</v>
+        <f t="shared" ref="A117:A129" ca="1" si="3">IF(OFFSET(A117,-1,0) ="",OFFSET(A117,-2,0)+1,OFFSET(A117,-1,0)+1 )</f>
+        <v>74</v>
       </c>
       <c r="B117" s="51"/>
       <c r="C117" s="51"/>
       <c r="D117" s="53"/>
-      <c r="E117" s="59"/>
+      <c r="E117" s="53"/>
       <c r="F117" s="51"/>
       <c r="G117" s="51"/>
       <c r="H117" s="51"/>
@@ -6417,8 +6422,8 @@
     </row>
     <row r="118" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A118" s="61">
-        <f t="shared" ca="1" si="2"/>
-        <v>76</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>75</v>
       </c>
       <c r="B118" s="51"/>
       <c r="C118" s="51"/>
@@ -6431,8 +6436,8 @@
     </row>
     <row r="119" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A119" s="61">
-        <f t="shared" ca="1" si="2"/>
-        <v>77</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>76</v>
       </c>
       <c r="B119" s="51"/>
       <c r="C119" s="51"/>
@@ -6445,8 +6450,8 @@
     </row>
     <row r="120" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A120" s="61">
-        <f t="shared" ca="1" si="2"/>
-        <v>78</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>77</v>
       </c>
       <c r="B120" s="51"/>
       <c r="C120" s="51"/>
@@ -6459,8 +6464,8 @@
     </row>
     <row r="121" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A121" s="61">
-        <f t="shared" ca="1" si="2"/>
-        <v>79</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>78</v>
       </c>
       <c r="B121" s="51"/>
       <c r="C121" s="51"/>
@@ -6473,8 +6478,8 @@
     </row>
     <row r="122" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A122" s="61">
-        <f t="shared" ca="1" si="2"/>
-        <v>80</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>79</v>
       </c>
       <c r="B122" s="51"/>
       <c r="C122" s="51"/>
@@ -6487,8 +6492,8 @@
     </row>
     <row r="123" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A123" s="61">
-        <f t="shared" ca="1" si="2"/>
-        <v>81</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>80</v>
       </c>
       <c r="B123" s="51"/>
       <c r="C123" s="51"/>
@@ -6501,8 +6506,8 @@
     </row>
     <row r="124" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A124" s="61">
-        <f t="shared" ca="1" si="2"/>
-        <v>82</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>81</v>
       </c>
       <c r="B124" s="51"/>
       <c r="C124" s="51"/>
@@ -6515,8 +6520,8 @@
     </row>
     <row r="125" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A125" s="61">
-        <f t="shared" ca="1" si="2"/>
-        <v>83</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>82</v>
       </c>
       <c r="B125" s="51"/>
       <c r="C125" s="51"/>
@@ -6529,8 +6534,8 @@
     </row>
     <row r="126" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A126" s="61">
-        <f t="shared" ca="1" si="2"/>
-        <v>84</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>83</v>
       </c>
       <c r="B126" s="51"/>
       <c r="C126" s="51"/>
@@ -6543,8 +6548,8 @@
     </row>
     <row r="127" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A127" s="61">
-        <f t="shared" ca="1" si="2"/>
-        <v>85</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>84</v>
       </c>
       <c r="B127" s="51"/>
       <c r="C127" s="51"/>
@@ -6557,98 +6562,98 @@
     </row>
     <row r="128" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A128" s="61">
-        <f t="shared" ca="1" si="2"/>
-        <v>86</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>85</v>
       </c>
       <c r="B128" s="51"/>
-      <c r="C128" s="167"/>
-      <c r="D128" s="168"/>
+      <c r="C128" s="51"/>
+      <c r="D128" s="53"/>
       <c r="E128" s="59"/>
       <c r="F128" s="51"/>
       <c r="G128" s="51"/>
       <c r="H128" s="51"/>
       <c r="I128" s="61"/>
     </row>
-    <row r="129" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B129" s="162"/>
-      <c r="C129" s="163"/>
-      <c r="D129" s="164"/>
-      <c r="E129" s="162"/>
-      <c r="F129" s="165"/>
-      <c r="G129" s="165"/>
-      <c r="H129" s="165"/>
-      <c r="I129" s="162"/>
-    </row>
-    <row r="130" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A130" s="61">
-        <f t="shared" ca="1" si="0"/>
+    <row r="129" spans="1:9" s="48" customFormat="1" ht="14.25">
+      <c r="A129" s="61">
+        <f t="shared" ca="1" si="3"/>
+        <v>86</v>
+      </c>
+      <c r="B129" s="51"/>
+      <c r="C129" s="167"/>
+      <c r="D129" s="168"/>
+      <c r="E129" s="59"/>
+      <c r="F129" s="51"/>
+      <c r="G129" s="51"/>
+      <c r="H129" s="51"/>
+      <c r="I129" s="61"/>
+    </row>
+    <row r="130" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B130" s="162"/>
+      <c r="C130" s="163"/>
+      <c r="D130" s="164"/>
+      <c r="E130" s="162"/>
+      <c r="F130" s="165"/>
+      <c r="G130" s="165"/>
+      <c r="H130" s="165"/>
+      <c r="I130" s="162"/>
+    </row>
+    <row r="131" spans="1:9" s="48" customFormat="1" ht="14.25">
+      <c r="A131" s="61">
+        <f t="shared" ca="1" si="1"/>
         <v>87</v>
       </c>
-      <c r="B130" s="51"/>
-      <c r="C130" s="51"/>
-      <c r="D130" s="52"/>
-      <c r="E130" s="53"/>
-      <c r="F130" s="51"/>
-      <c r="G130" s="51"/>
-      <c r="H130" s="51"/>
-      <c r="I130" s="61"/>
-    </row>
-    <row r="131" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B131" s="162"/>
-      <c r="C131" s="163"/>
-      <c r="D131" s="164"/>
-      <c r="E131" s="162"/>
-      <c r="F131" s="165"/>
-      <c r="G131" s="165"/>
-      <c r="H131" s="165"/>
-      <c r="I131" s="162"/>
-    </row>
-    <row r="132" spans="1:9" s="48" customFormat="1" ht="30" customHeight="1">
-      <c r="A132" s="61">
-        <f t="shared" ca="1" si="0"/>
+      <c r="B131" s="51"/>
+      <c r="C131" s="51"/>
+      <c r="D131" s="52"/>
+      <c r="E131" s="53"/>
+      <c r="F131" s="51"/>
+      <c r="G131" s="51"/>
+      <c r="H131" s="51"/>
+      <c r="I131" s="61"/>
+    </row>
+    <row r="132" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B132" s="162"/>
+      <c r="C132" s="163"/>
+      <c r="D132" s="164"/>
+      <c r="E132" s="162"/>
+      <c r="F132" s="165"/>
+      <c r="G132" s="165"/>
+      <c r="H132" s="165"/>
+      <c r="I132" s="162"/>
+    </row>
+    <row r="133" spans="1:9" s="48" customFormat="1" ht="30" customHeight="1">
+      <c r="A133" s="61">
+        <f t="shared" ca="1" si="1"/>
         <v>88</v>
       </c>
-      <c r="B132" s="51"/>
-      <c r="C132" s="51"/>
-      <c r="D132" s="58"/>
-      <c r="E132" s="53"/>
-      <c r="F132" s="51"/>
-      <c r="G132" s="51"/>
-      <c r="H132" s="51"/>
-      <c r="I132" s="61"/>
-    </row>
-    <row r="133" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B133" s="162"/>
-      <c r="C133" s="163"/>
-      <c r="D133" s="164"/>
-      <c r="E133" s="162"/>
-      <c r="F133" s="165"/>
-      <c r="G133" s="165"/>
-      <c r="H133" s="165"/>
-      <c r="I133" s="162"/>
-    </row>
-    <row r="134" spans="1:9" s="48" customFormat="1" ht="14.25">
-      <c r="A134" s="61">
-        <f t="shared" ca="1" si="0"/>
-        <v>89</v>
-      </c>
-      <c r="B134" s="51"/>
-      <c r="C134" s="51"/>
-      <c r="D134" s="52"/>
-      <c r="E134" s="53"/>
-      <c r="F134" s="51"/>
-      <c r="G134" s="51"/>
-      <c r="H134" s="51"/>
-      <c r="I134" s="61"/>
+      <c r="B133" s="51"/>
+      <c r="C133" s="51"/>
+      <c r="D133" s="58"/>
+      <c r="E133" s="53"/>
+      <c r="F133" s="51"/>
+      <c r="G133" s="51"/>
+      <c r="H133" s="51"/>
+      <c r="I133" s="61"/>
+    </row>
+    <row r="134" spans="1:9" s="166" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B134" s="162"/>
+      <c r="C134" s="163"/>
+      <c r="D134" s="164"/>
+      <c r="E134" s="162"/>
+      <c r="F134" s="165"/>
+      <c r="G134" s="165"/>
+      <c r="H134" s="165"/>
+      <c r="I134" s="162"/>
     </row>
     <row r="135" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A135" s="61">
-        <f t="shared" ca="1" si="0"/>
-        <v>90</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>89</v>
       </c>
       <c r="B135" s="51"/>
       <c r="C135" s="51"/>
-      <c r="D135" s="59"/>
+      <c r="D135" s="52"/>
       <c r="E135" s="53"/>
       <c r="F135" s="51"/>
       <c r="G135" s="51"/>
@@ -6657,12 +6662,12 @@
     </row>
     <row r="136" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A136" s="61">
-        <f t="shared" ref="A136:A143" ca="1" si="3">IF(OFFSET(A136,-1,0) ="",OFFSET(A136,-2,0)+1,OFFSET(A136,-1,0)+1 )</f>
-        <v>91</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>90</v>
       </c>
       <c r="B136" s="51"/>
       <c r="C136" s="51"/>
-      <c r="D136" s="53"/>
+      <c r="D136" s="59"/>
       <c r="E136" s="53"/>
       <c r="F136" s="51"/>
       <c r="G136" s="51"/>
@@ -6671,13 +6676,13 @@
     </row>
     <row r="137" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A137" s="61">
-        <f t="shared" ca="1" si="3"/>
-        <v>92</v>
+        <f t="shared" ref="A137:A144" ca="1" si="4">IF(OFFSET(A137,-1,0) ="",OFFSET(A137,-2,0)+1,OFFSET(A137,-1,0)+1 )</f>
+        <v>91</v>
       </c>
       <c r="B137" s="51"/>
       <c r="C137" s="51"/>
       <c r="D137" s="53"/>
-      <c r="E137" s="59"/>
+      <c r="E137" s="53"/>
       <c r="F137" s="51"/>
       <c r="G137" s="51"/>
       <c r="H137" s="51"/>
@@ -6685,12 +6690,12 @@
     </row>
     <row r="138" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A138" s="61">
-        <f t="shared" ca="1" si="3"/>
-        <v>93</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>92</v>
       </c>
       <c r="B138" s="51"/>
       <c r="C138" s="51"/>
-      <c r="D138" s="59"/>
+      <c r="D138" s="53"/>
       <c r="E138" s="59"/>
       <c r="F138" s="51"/>
       <c r="G138" s="51"/>
@@ -6699,13 +6704,13 @@
     </row>
     <row r="139" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A139" s="61">
-        <f t="shared" ca="1" si="3"/>
-        <v>94</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>93</v>
       </c>
       <c r="B139" s="51"/>
       <c r="C139" s="51"/>
-      <c r="D139" s="52"/>
-      <c r="E139" s="53"/>
+      <c r="D139" s="59"/>
+      <c r="E139" s="59"/>
       <c r="F139" s="51"/>
       <c r="G139" s="51"/>
       <c r="H139" s="51"/>
@@ -6713,12 +6718,12 @@
     </row>
     <row r="140" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A140" s="61">
-        <f t="shared" ca="1" si="3"/>
-        <v>95</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>94</v>
       </c>
       <c r="B140" s="51"/>
       <c r="C140" s="51"/>
-      <c r="D140" s="59"/>
+      <c r="D140" s="52"/>
       <c r="E140" s="53"/>
       <c r="F140" s="51"/>
       <c r="G140" s="51"/>
@@ -6727,8 +6732,8 @@
     </row>
     <row r="141" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A141" s="61">
-        <f t="shared" ca="1" si="3"/>
-        <v>96</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>95</v>
       </c>
       <c r="B141" s="51"/>
       <c r="C141" s="51"/>
@@ -6741,8 +6746,8 @@
     </row>
     <row r="142" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A142" s="61">
-        <f t="shared" ca="1" si="3"/>
-        <v>97</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>96</v>
       </c>
       <c r="B142" s="51"/>
       <c r="C142" s="51"/>
@@ -6755,8 +6760,8 @@
     </row>
     <row r="143" spans="1:9" s="48" customFormat="1" ht="14.25">
       <c r="A143" s="61">
-        <f t="shared" ca="1" si="3"/>
-        <v>98</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>97</v>
       </c>
       <c r="B143" s="51"/>
       <c r="C143" s="51"/>
@@ -6767,30 +6772,44 @@
       <c r="H143" s="51"/>
       <c r="I143" s="61"/>
     </row>
+    <row r="144" spans="1:9" s="48" customFormat="1" ht="14.25">
+      <c r="A144" s="61">
+        <f t="shared" ca="1" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="B144" s="51"/>
+      <c r="C144" s="51"/>
+      <c r="D144" s="59"/>
+      <c r="E144" s="53"/>
+      <c r="F144" s="51"/>
+      <c r="G144" s="51"/>
+      <c r="H144" s="51"/>
+      <c r="I144" s="61"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="B6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B8:D8"/>
     <mergeCell ref="F16:H16"/>
     <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B113:D113"/>
+    <mergeCell ref="B114:D114"/>
     <mergeCell ref="E2:E3"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="B18:D18"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="B6:D6"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation showDropDown="1" showErrorMessage="1" sqref="F16:H17"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:H19 F129:H129 F114:H114 F87:H87 F95:H96 F109:H109 F131:H131 F133:H133 F69:H69"/>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F144:H201">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F18:H19 F130:H130 F115:H115 F88:H88 F96:H97 F110:H110 F132:H132 F134:H134 F70:H70"/>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F145:H202">
       <formula1>#REF!</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F110:H113 F88:H94 F130:H130 F132:H132 F134:H143 F70:H86 F97:H108 F115:H128 F20:H68">
+    <dataValidation type="list" allowBlank="1" sqref="F111:H114 F89:H95 F131:H131 F133:H133 F135:H144 F71:H87 F98:H109 F116:H129 F20:H69">
       <formula1>$A$11:$A$15</formula1>
     </dataValidation>
   </dataValidations>
@@ -6838,13 +6857,13 @@
     </row>
     <row r="2" spans="1:12" s="80" customFormat="1" ht="26.25">
       <c r="A2" s="79"/>
-      <c r="C2" s="214" t="s">
+      <c r="C2" s="232" t="s">
         <v>114</v>
       </c>
-      <c r="D2" s="214"/>
-      <c r="E2" s="214"/>
-      <c r="F2" s="214"/>
-      <c r="G2" s="214"/>
+      <c r="D2" s="232"/>
+      <c r="E2" s="232"/>
+      <c r="F2" s="232"/>
+      <c r="G2" s="232"/>
       <c r="H2" s="81" t="s">
         <v>115</v>
       </c>
@@ -6855,15 +6874,15 @@
     </row>
     <row r="3" spans="1:12" s="80" customFormat="1" ht="23.25">
       <c r="A3" s="79"/>
-      <c r="C3" s="215" t="s">
+      <c r="C3" s="233" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="215"/>
+      <c r="D3" s="233"/>
       <c r="E3" s="152"/>
-      <c r="F3" s="216" t="s">
+      <c r="F3" s="234" t="s">
         <v>117</v>
       </c>
-      <c r="G3" s="216"/>
+      <c r="G3" s="234"/>
       <c r="H3" s="82"/>
       <c r="I3" s="82"/>
       <c r="J3" s="83"/>
@@ -6888,10 +6907,10 @@
       <c r="L5" s="88"/>
     </row>
     <row r="6" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B6" s="217" t="s">
+      <c r="B6" s="216" t="s">
         <v>118</v>
       </c>
-      <c r="C6" s="217"/>
+      <c r="C6" s="216"/>
       <c r="D6" s="90"/>
       <c r="E6" s="90"/>
       <c r="F6" s="90"/>
@@ -7060,11 +7079,11 @@
       <c r="G13" s="94"/>
     </row>
     <row r="14" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B14" s="217" t="s">
+      <c r="B14" s="216" t="s">
         <v>148</v>
       </c>
-      <c r="C14" s="217"/>
-      <c r="D14" s="217"/>
+      <c r="C14" s="216"/>
+      <c r="D14" s="216"/>
       <c r="E14" s="90"/>
       <c r="F14" s="90"/>
       <c r="G14" s="91"/>
@@ -7240,11 +7259,11 @@
       <c r="G22" s="94"/>
     </row>
     <row r="23" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B23" s="217" t="s">
+      <c r="B23" s="216" t="s">
         <v>158</v>
       </c>
-      <c r="C23" s="217"/>
-      <c r="D23" s="217"/>
+      <c r="C23" s="216"/>
+      <c r="D23" s="216"/>
       <c r="E23" s="90"/>
       <c r="F23" s="90"/>
       <c r="G23" s="91"/>
@@ -7290,10 +7309,10 @@
       <c r="F26" s="155" t="s">
         <v>165</v>
       </c>
-      <c r="G26" s="218" t="s">
+      <c r="G26" s="235" t="s">
         <v>110</v>
       </c>
-      <c r="H26" s="219"/>
+      <c r="H26" s="236"/>
     </row>
     <row r="27" spans="1:12">
       <c r="A27" s="96">
@@ -7318,8 +7337,8 @@
         <f>COUNTIFS(#REF!, "*Critical*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Critical*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G27" s="212"/>
-      <c r="H27" s="213"/>
+      <c r="G27" s="227"/>
+      <c r="H27" s="228"/>
     </row>
     <row r="28" spans="1:12" ht="20.25" customHeight="1">
       <c r="A28" s="96">
@@ -7344,8 +7363,8 @@
         <f>COUNTIFS(#REF!, "*Major*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Major*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G28" s="212"/>
-      <c r="H28" s="213"/>
+      <c r="G28" s="227"/>
+      <c r="H28" s="228"/>
     </row>
     <row r="29" spans="1:12" ht="20.25" customHeight="1">
       <c r="A29" s="96">
@@ -7370,8 +7389,8 @@
         <f>COUNTIFS(#REF!, "*Normal*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Normal*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G29" s="212"/>
-      <c r="H29" s="213"/>
+      <c r="G29" s="227"/>
+      <c r="H29" s="228"/>
     </row>
     <row r="30" spans="1:12" ht="20.25" customHeight="1">
       <c r="A30" s="96">
@@ -7396,8 +7415,8 @@
         <f>COUNTIFS(#REF!, "*Minor*",#REF!,"*Closed*") + COUNTIFS(#REF!, "*Minor*",#REF!,"*Ready for client test*")</f>
         <v>#REF!</v>
       </c>
-      <c r="G30" s="212"/>
-      <c r="H30" s="213"/>
+      <c r="G30" s="227"/>
+      <c r="H30" s="228"/>
     </row>
     <row r="31" spans="1:12" ht="20.25" customHeight="1">
       <c r="A31" s="96"/>
@@ -7418,8 +7437,8 @@
         <f>SUM(F27:F30)</f>
         <v>#REF!</v>
       </c>
-      <c r="G31" s="212"/>
-      <c r="H31" s="213"/>
+      <c r="G31" s="227"/>
+      <c r="H31" s="228"/>
     </row>
     <row r="32" spans="1:12" ht="20.25" customHeight="1">
       <c r="A32" s="102"/>
@@ -7457,10 +7476,10 @@
       <c r="E34" s="155" t="s">
         <v>124</v>
       </c>
-      <c r="F34" s="220" t="s">
+      <c r="F34" s="221" t="s">
         <v>127</v>
       </c>
-      <c r="G34" s="221"/>
+      <c r="G34" s="223"/>
     </row>
     <row r="35" spans="1:12" s="121" customFormat="1">
       <c r="A35" s="117"/>
@@ -7476,8 +7495,8 @@
       <c r="E35" s="122" t="s">
         <v>132</v>
       </c>
-      <c r="F35" s="223"/>
-      <c r="G35" s="224"/>
+      <c r="F35" s="230"/>
+      <c r="G35" s="231"/>
       <c r="H35" s="120"/>
       <c r="I35" s="120"/>
       <c r="J35" s="120"/>
@@ -7500,8 +7519,8 @@
       <c r="E36" s="100" t="s">
         <v>138</v>
       </c>
-      <c r="F36" s="212"/>
-      <c r="G36" s="213"/>
+      <c r="F36" s="227"/>
+      <c r="G36" s="228"/>
     </row>
     <row r="37" spans="1:12" ht="20.25" customHeight="1">
       <c r="A37" s="96">
@@ -7519,8 +7538,8 @@
       <c r="E37" s="100" t="s">
         <v>138</v>
       </c>
-      <c r="F37" s="212"/>
-      <c r="G37" s="213"/>
+      <c r="F37" s="227"/>
+      <c r="G37" s="228"/>
     </row>
     <row r="38" spans="1:12" ht="20.25" customHeight="1">
       <c r="A38" s="102"/>
@@ -7533,10 +7552,10 @@
       <c r="H38" s="104"/>
     </row>
     <row r="39" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B39" s="217" t="s">
+      <c r="B39" s="216" t="s">
         <v>179</v>
       </c>
-      <c r="C39" s="217"/>
+      <c r="C39" s="216"/>
       <c r="D39" s="90"/>
       <c r="E39" s="90"/>
       <c r="F39" s="90"/>
@@ -7560,15 +7579,15 @@
       <c r="B41" s="155" t="s">
         <v>62</v>
       </c>
-      <c r="C41" s="222" t="s">
+      <c r="C41" s="229" t="s">
         <v>181</v>
       </c>
-      <c r="D41" s="222"/>
-      <c r="E41" s="222" t="s">
+      <c r="D41" s="229"/>
+      <c r="E41" s="229" t="s">
         <v>182</v>
       </c>
-      <c r="F41" s="222"/>
-      <c r="G41" s="222"/>
+      <c r="F41" s="229"/>
+      <c r="G41" s="229"/>
       <c r="H41" s="95" t="s">
         <v>183</v>
       </c>
@@ -7580,15 +7599,15 @@
       <c r="B42" s="156" t="s">
         <v>184</v>
       </c>
-      <c r="C42" s="225" t="s">
+      <c r="C42" s="226" t="s">
         <v>185</v>
       </c>
-      <c r="D42" s="225"/>
-      <c r="E42" s="225" t="s">
+      <c r="D42" s="226"/>
+      <c r="E42" s="226" t="s">
         <v>186</v>
       </c>
-      <c r="F42" s="225"/>
-      <c r="G42" s="225"/>
+      <c r="F42" s="226"/>
+      <c r="G42" s="226"/>
       <c r="H42" s="105"/>
     </row>
     <row r="43" spans="1:12" ht="34.5" customHeight="1">
@@ -7598,15 +7617,15 @@
       <c r="B43" s="156" t="s">
         <v>184</v>
       </c>
-      <c r="C43" s="225" t="s">
+      <c r="C43" s="226" t="s">
         <v>185</v>
       </c>
-      <c r="D43" s="225"/>
-      <c r="E43" s="225" t="s">
+      <c r="D43" s="226"/>
+      <c r="E43" s="226" t="s">
         <v>186</v>
       </c>
-      <c r="F43" s="225"/>
-      <c r="G43" s="225"/>
+      <c r="F43" s="226"/>
+      <c r="G43" s="226"/>
       <c r="H43" s="105"/>
     </row>
     <row r="44" spans="1:12" ht="34.5" customHeight="1">
@@ -7616,15 +7635,15 @@
       <c r="B44" s="156" t="s">
         <v>184</v>
       </c>
-      <c r="C44" s="225" t="s">
+      <c r="C44" s="226" t="s">
         <v>185</v>
       </c>
-      <c r="D44" s="225"/>
-      <c r="E44" s="225" t="s">
+      <c r="D44" s="226"/>
+      <c r="E44" s="226" t="s">
         <v>186</v>
       </c>
-      <c r="F44" s="225"/>
-      <c r="G44" s="225"/>
+      <c r="F44" s="226"/>
+      <c r="G44" s="226"/>
       <c r="H44" s="105"/>
     </row>
     <row r="45" spans="1:12">
@@ -7636,10 +7655,10 @@
       <c r="G45" s="94"/>
     </row>
     <row r="46" spans="1:12" ht="21.75" customHeight="1">
-      <c r="B46" s="217" t="s">
+      <c r="B46" s="216" t="s">
         <v>187</v>
       </c>
-      <c r="C46" s="217"/>
+      <c r="C46" s="216"/>
       <c r="D46" s="90"/>
       <c r="E46" s="90"/>
       <c r="F46" s="90"/>
@@ -7657,25 +7676,25 @@
       <c r="G47" s="94"/>
     </row>
     <row r="48" spans="1:12" s="109" customFormat="1" ht="21" customHeight="1">
-      <c r="A48" s="228" t="s">
+      <c r="A48" s="217" t="s">
         <v>58</v>
       </c>
-      <c r="B48" s="230" t="s">
+      <c r="B48" s="219" t="s">
         <v>189</v>
       </c>
-      <c r="C48" s="220" t="s">
+      <c r="C48" s="221" t="s">
         <v>190</v>
       </c>
-      <c r="D48" s="232"/>
-      <c r="E48" s="232"/>
-      <c r="F48" s="221"/>
-      <c r="G48" s="233" t="s">
+      <c r="D48" s="222"/>
+      <c r="E48" s="222"/>
+      <c r="F48" s="223"/>
+      <c r="G48" s="224" t="s">
         <v>157</v>
       </c>
-      <c r="H48" s="233" t="s">
+      <c r="H48" s="224" t="s">
         <v>189</v>
       </c>
-      <c r="I48" s="226" t="s">
+      <c r="I48" s="214" t="s">
         <v>191</v>
       </c>
       <c r="J48" s="108"/>
@@ -7683,8 +7702,8 @@
       <c r="L48" s="108"/>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="229"/>
-      <c r="B49" s="231"/>
+      <c r="A49" s="218"/>
+      <c r="B49" s="220"/>
       <c r="C49" s="110" t="s">
         <v>166</v>
       </c>
@@ -7697,13 +7716,13 @@
       <c r="F49" s="111" t="s">
         <v>169</v>
       </c>
-      <c r="G49" s="234"/>
-      <c r="H49" s="234"/>
-      <c r="I49" s="227"/>
+      <c r="G49" s="225"/>
+      <c r="H49" s="225"/>
+      <c r="I49" s="215"/>
     </row>
     <row r="50" spans="1:9" ht="38.25">
-      <c r="A50" s="229"/>
-      <c r="B50" s="231"/>
+      <c r="A50" s="218"/>
+      <c r="B50" s="220"/>
       <c r="C50" s="124" t="s">
         <v>192</v>
       </c>
@@ -7815,26 +7834,6 @@
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="I48:I49"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="A48:A50"/>
-    <mergeCell ref="B48:B50"/>
-    <mergeCell ref="C48:F48"/>
-    <mergeCell ref="G48:G49"/>
-    <mergeCell ref="H48:H49"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="E42:G42"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="E44:G44"/>
-    <mergeCell ref="F34:G34"/>
-    <mergeCell ref="F36:G36"/>
-    <mergeCell ref="F37:G37"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="F35:G35"/>
     <mergeCell ref="G31:H31"/>
     <mergeCell ref="C2:G2"/>
     <mergeCell ref="C3:D3"/>
@@ -7847,6 +7846,26 @@
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G30:H30"/>
+    <mergeCell ref="F34:G34"/>
+    <mergeCell ref="F36:G36"/>
+    <mergeCell ref="F37:G37"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="C42:D42"/>
+    <mergeCell ref="E42:G42"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="E44:G44"/>
+    <mergeCell ref="I48:I49"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A48:A50"/>
+    <mergeCell ref="B48:B50"/>
+    <mergeCell ref="C48:F48"/>
+    <mergeCell ref="G48:G49"/>
+    <mergeCell ref="H48:H49"/>
   </mergeCells>
   <conditionalFormatting sqref="H51">
     <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
@@ -8049,18 +8068,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8083,14 +8102,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F8C6C6D-E626-49D4-9BA8-E27B2B9C9191}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{06E3E4FA-795A-4742-A021-9CDC3210C50B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -8105,4 +8116,12 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4F8C6C6D-E626-49D4-9BA8-E27B2B9C9191}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>